<commit_message>
changed process handling for MQTT python script
</commit_message>
<xml_diff>
--- a/MQTT_Metrics.xlsx
+++ b/MQTT_Metrics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kollm\source\repos\WateringOS_3_0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F726845A-3675-4DE0-9B75-7283B7F7A59D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85AE36AE-D745-490B-BE9A-5FA44D5A28AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{11DDC7D6-ACEA-4B69-8CE7-26A9FB692193}"/>
   </bookViews>
@@ -734,7 +734,7 @@
   <dimension ref="B3:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1074,7 +1074,7 @@
       <c r="D15" t="s">
         <v>59</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15">
         <v>1</v>
       </c>
       <c r="G15" t="s">

</xml_diff>

<commit_message>
- added loading animation to all chart pages - corrected loading of version number from txt
</commit_message>
<xml_diff>
--- a/MQTT_Metrics.xlsx
+++ b/MQTT_Metrics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kollm\source\repos\WateringOS_3_0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85AE36AE-D745-490B-BE9A-5FA44D5A28AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4587FE1-35A7-4D4C-918A-1297CF377FF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{11DDC7D6-ACEA-4B69-8CE7-26A9FB692193}"/>
+    <workbookView xWindow="4470" yWindow="3735" windowWidth="28800" windowHeight="15435" xr2:uid="{11DDC7D6-ACEA-4B69-8CE7-26A9FB692193}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -352,7 +352,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -381,13 +381,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -399,11 +411,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -416,8 +429,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -734,7 +749,7 @@
   <dimension ref="B3:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1298,164 +1313,164 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+    <row r="24" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D24" t="s">
-        <v>57</v>
-      </c>
-      <c r="F24" t="s">
-        <v>57</v>
-      </c>
-      <c r="H24">
+      <c r="D24" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H24" s="6">
         <v>21</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I24" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="J24" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+      <c r="J24" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D25" t="s">
-        <v>57</v>
-      </c>
-      <c r="F25" t="s">
-        <v>57</v>
-      </c>
-      <c r="H25">
+      <c r="D25" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H25" s="6">
         <v>22</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I25" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="J25" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+      <c r="J25" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D26" t="s">
-        <v>57</v>
-      </c>
-      <c r="F26" t="s">
-        <v>57</v>
-      </c>
-      <c r="H26">
+      <c r="D26" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H26" s="6">
         <v>23</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I26" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="J26" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+      <c r="J26" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D27" t="s">
-        <v>57</v>
-      </c>
-      <c r="F27" t="s">
-        <v>57</v>
-      </c>
-      <c r="H27">
+      <c r="D27" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H27" s="6">
         <v>24</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I27" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="J27" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+      <c r="J27" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D28" t="s">
-        <v>57</v>
-      </c>
-      <c r="F28" t="s">
-        <v>57</v>
-      </c>
-      <c r="H28">
+      <c r="D28" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H28" s="6">
         <v>25</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I28" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="J28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+      <c r="J28" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D29" t="s">
-        <v>57</v>
-      </c>
-      <c r="F29" t="s">
-        <v>57</v>
-      </c>
-      <c r="H29">
+      <c r="D29" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H29" s="6">
         <v>26</v>
       </c>
-      <c r="I29" t="s">
+      <c r="I29" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="J29" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+      <c r="J29" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F30" t="s">
-        <v>57</v>
-      </c>
-      <c r="H30">
+      <c r="D30" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H30" s="6">
         <v>27</v>
       </c>
-      <c r="I30" t="s">
+      <c r="I30" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="J30" t="s">
+      <c r="J30" s="6" t="s">
         <v>73</v>
       </c>
     </row>

</xml_diff>